<commit_message>
Revert "Merge branch 'main' of https://github.com/st-igoriy/GZ"
This reverts commit 17abcc913ba6e2e1caff0fe73d80882eb9b25c48, reversing
changes made to 11ead44058d35a5bd3726c3071dd0848d14506be.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647008E4-F19B-4EA1-A3D0-9ECADBFB2618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782CFAE3-E386-4334-924C-AEBB65E79818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14510" yWindow="-110" windowWidth="14620" windowHeight="25220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2712,7 +2712,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2742,7 +2742,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="10">
-        <v>15</v>
+        <v>-3.1</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>

</xml_diff>